<commit_message>
Split fugacity calculations into smaller generic chunks so that individual pieces of calculate_fugacities can be used elsewhere. Updated manual calculations for unittesting and updated the test_calculate method to do calcs at 926 to match spreadsheet. All tests passing.
</commit_message>
<xml_diff>
--- a/tests/Manual_Speciation_Calculation.xlsx
+++ b/tests/Manual_Speciation_Calculation.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Python/TAVERN/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Python/TAVERNmag/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FF051E-51B9-1A42-9FDE-BBB971CFBE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639BAA78-704D-C745-9154-438B44015BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="29480" windowWidth="33600" windowHeight="21720" activeTab="3" xr2:uid="{625D6B45-C922-FA47-8BB4-172CE4823A05}"/>
+    <workbookView xWindow="9680" yWindow="30000" windowWidth="33600" windowHeight="21720" activeTab="4" xr2:uid="{625D6B45-C922-FA47-8BB4-172CE4823A05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="logKs" sheetId="2" r:id="rId2"/>
     <sheet name="gammas" sheetId="4" r:id="rId3"/>
     <sheet name="fugacities" sheetId="3" r:id="rId4"/>
+    <sheet name="Speciation" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>H2O</t>
   </si>
@@ -237,6 +238,21 @@
   </si>
   <si>
     <t>KCO2 * fCO * sqrt(fO2)</t>
+  </si>
+  <si>
+    <t>mole fraction</t>
+  </si>
+  <si>
+    <t>norm_fix_ox</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>normsum</t>
+  </si>
+  <si>
+    <t>wt%</t>
   </si>
 </sst>
 </file>
@@ -298,13 +314,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -914,7 +929,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,66 +941,66 @@
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4">
-        <v>1.2702307224970899</v>
+        <v>1.19946588566002</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4">
-        <v>1.17702986434571</v>
+        <v>1.1995158606479099</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4">
-        <v>1.1995158606479099</v>
+        <v>1.16052802963702</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4">
-        <v>0.86908487374434096</v>
+        <v>1.2702307224970899</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B6" s="4">
-        <v>1.11989805891392</v>
+        <v>1.17702986434571</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4">
-        <v>1.19946588566002</v>
+        <v>1.12402533093521</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4">
-        <v>1.16052802963702</v>
+        <v>1.11989805891392</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B9" s="4">
-        <v>1.12402533093521</v>
+        <v>0.86908487374434096</v>
       </c>
     </row>
   </sheetData>
@@ -997,16 +1012,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64078AA3-0D68-694E-A696-73A02DF83B1E}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="60.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1041,11 +1056,11 @@
         <f>10^-11.101768</f>
         <v>7.9110112115639112E-12</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>7.9110164857329103E-12</v>
       </c>
-      <c r="E2" s="6">
-        <f>C2-D2</f>
+      <c r="E2" s="5">
+        <f t="shared" ref="E2:E9" si="0">C2-D2</f>
         <v>-5.2741689991455686E-18</v>
       </c>
       <c r="G2" t="s">
@@ -1066,11 +1081,11 @@
       <c r="C3">
         <v>7.2968500000000001</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>7.2969344854999996</v>
       </c>
-      <c r="E3" s="6">
-        <f>C3-D3</f>
+      <c r="E3" s="5">
+        <f t="shared" si="0"/>
         <v>-8.4485499999509273E-5</v>
       </c>
     </row>
@@ -1084,11 +1099,11 @@
       <c r="C4">
         <v>4.9765600000000001</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>4.9764539578000004</v>
       </c>
-      <c r="E4" s="6">
-        <f>C4-D4</f>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
         <v>1.0604219999965636E-4</v>
       </c>
       <c r="G4" t="s">
@@ -1105,11 +1120,11 @@
       <c r="C5">
         <v>4.26919</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>4.26918839299986</v>
       </c>
-      <c r="E5" s="6">
-        <f>C5-D5</f>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
         <v>1.6070001400692036E-6</v>
       </c>
       <c r="G5" t="s">
@@ -1127,11 +1142,11 @@
         <f>logKs!C2*fugacities!C5*SQRT(fugacities!C2)</f>
         <v>713.52323509945336</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>713.52320436466903</v>
       </c>
-      <c r="E6" s="6">
-        <f>C6-D6</f>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
         <v>3.0734784331798437E-5</v>
       </c>
       <c r="G6" t="s">
@@ -1149,11 +1164,11 @@
         <f>logKs!C5*SQRT(fugacities!C4)*fugacities!C2</f>
         <v>14.220786157682392</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>14.220644126961901</v>
       </c>
-      <c r="E7" s="6">
-        <f>C7-D7</f>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
         <v>1.4203072049134846E-4</v>
       </c>
     </row>
@@ -1168,11 +1183,11 @@
         <f>logKs!C4*fugacities!C3*SQRT(fugacities!C4)</f>
         <v>400.92928173572443</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>400.92965219656799</v>
       </c>
-      <c r="E8" s="6">
-        <f>C8-D8</f>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
         <v>-3.7046084355552011E-4</v>
       </c>
       <c r="G8" t="s">
@@ -1190,11 +1205,11 @@
         <f>logKs!C3*SQRT(fugacities!C2)*fugacities!C3</f>
         <v>1423.631304082651</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>1423.6482619511501</v>
       </c>
-      <c r="E9" s="6">
-        <f>C9-D9</f>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
         <v>-1.6957868499048345E-2</v>
       </c>
       <c r="G9" t="s">
@@ -1230,4 +1245,265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535B0DA0-D69E-434D-AC2B-4AB05E3AB8D3}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <f>fugacities!C2/(gammas!B2*Sheet1!$B$9)</f>
+        <v>6.595444944406056E-15</v>
+      </c>
+      <c r="C2">
+        <f>B2</f>
+        <v>6.595444944406056E-15</v>
+      </c>
+      <c r="D2">
+        <f>2*15.999</f>
+        <v>31.998000000000001</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>2.1104104733110499E-13</v>
+      </c>
+      <c r="F2">
+        <f>100*E2/E$11</f>
+        <v>7.9750001009541675E-13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <f>fugacities!C3/(gammas!B3*Sheet1!$B$9)</f>
+        <v>6.0831625819925874E-3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C9" si="0">B3/B$12*(1-B$2)</f>
+        <v>2.3141540791191744E-3</v>
+      </c>
+      <c r="D3">
+        <f>2.016</f>
+        <v>2.016</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="1">C3*D3</f>
+        <v>4.6653346235042553E-3</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="2">100*E3/E$11</f>
+        <v>1.7629766608890249E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <f>fugacities!C4/(gammas!B4*Sheet1!$B$9)</f>
+        <v>4.2881859575218759E-3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1.6313098477749853E-3</v>
+      </c>
+      <c r="D4">
+        <f>2*32.065</f>
+        <v>64.13</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0.10461590053780979</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>0.39533153758542611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <f>fugacities!C5/(gammas!B5*Sheet1!$B$9)</f>
+        <v>3.3609563399690022E-3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.2785735575939594E-3</v>
+      </c>
+      <c r="D5">
+        <f>20.01</f>
+        <v>20.010000000000002</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2.558425688745513E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>9.6679984221353751E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f>fugacities!C6/(gammas!B6*Sheet1!$B$9)</f>
+        <v>0.60620656851055199</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.23061284067275661</v>
+      </c>
+      <c r="D6">
+        <v>44.01</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>10.149271118008018</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>38.352936177262556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>fugacities!C7/(gammas!B7*Sheet1!$B$9)</f>
+        <v>1.2651659857034035E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4.8129389723122317E-3</v>
+      </c>
+      <c r="D7">
+        <v>64.066000000000003</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0.30834574820015542</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>1.1652033593099931</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <f>fugacities!C8/(gammas!B8*Sheet1!$B$9)</f>
+        <v>0.35800515818783241</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.13619216747856555</v>
+      </c>
+      <c r="D8">
+        <v>34.1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>4.6441529110190851</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>17.549723337051006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <f>fugacities!C9/(gammas!B9*Sheet1!$B$9)</f>
+        <v>1.638080867693759</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.62315801539187077</v>
+      </c>
+      <c r="D9">
+        <v>18.015000000000001</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>11.226191647284553</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>42.422495837959971</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B2:B9)</f>
+        <v>2.6286765591286674</v>
+      </c>
+      <c r="C11">
+        <f>SUM(C2:C9)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E11">
+        <f>SUM(E2:E9)</f>
+        <v>26.462826916560793</v>
+      </c>
+      <c r="F11">
+        <f>SUM(F2:F9)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B3:B9)</f>
+        <v>2.6286765591286612</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>